<commit_message>
updated with ruby multi-pumping report
</commit_message>
<xml_diff>
--- a/assets/data/multipumping.xlsx
+++ b/assets/data/multipumping.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Coding/Research/ImperialSummerReports/assets/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RZ3515\Documents\GitHub\ImperialSummerReports\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="460" windowWidth="27740" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="1065" yWindow="465" windowWidth="27735" windowHeight="17535" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ROMRead-WindowSummation" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>C</t>
   </si>
@@ -46,10 +46,6 @@
   <si>
     <t>Time
 (us)</t>
-  </si>
-  <si>
-    <t>Freq
-(MHz)</t>
   </si>
   <si>
     <t>Bandwidth
@@ -155,12 +151,23 @@
   <si>
     <t>205(9.63%)</t>
   </si>
+  <si>
+    <t>FAILED TO MEET TIMING!</t>
+  </si>
+  <si>
+    <t>Freq per elem
+(MHz)</t>
+  </si>
+  <si>
+    <t>Freq per tick
+(MHz)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -185,6 +192,13 @@
       <color rgb="FFFF0000"/>
       <name val="Consolas"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -222,25 +236,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -250,6 +267,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -518,333 +538,372 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:I15"/>
+  <dimension ref="A3:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="3.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" customWidth="1"/>
+    <col min="2" max="3" width="3.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" customWidth="1"/>
+    <col min="8" max="9" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="3" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="4" t="s">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <f>8192*8192</f>
         <v>67108864</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>1</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="2">
         <v>4</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="6">
+      <c r="G6" s="2">
+        <v>2.9940000000000001E-3</v>
+      </c>
+      <c r="H6" s="2">
+        <v>83.51</v>
+      </c>
+      <c r="I6" s="2">
+        <v>333.96</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1335.84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="2">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2">
         <v>0</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="6">
-        <v>2.9940000000000001E-3</v>
-      </c>
-      <c r="H6" s="6">
-        <v>333.96</v>
-      </c>
-      <c r="I6" s="6">
-        <v>1335.84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6">
+      <c r="F7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="2">
+        <v>3.0869999999999999E-3</v>
+      </c>
+      <c r="H7" s="2">
+        <v>40.369999999999997</v>
+      </c>
+      <c r="I7" s="2">
+        <v>323.97000000000003</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1295.8800000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="2">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="2">
+        <v>3.3930000000000002E-3</v>
+      </c>
+      <c r="H8" s="2">
+        <v>18.45</v>
+      </c>
+      <c r="I8" s="2">
+        <v>294.7</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1178.81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="2">
+        <v>32</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="2">
+        <v>4.0819999999999997E-3</v>
+      </c>
+      <c r="H9" s="2">
+        <v>7.67</v>
+      </c>
+      <c r="I9" s="2">
+        <v>244.99</v>
+      </c>
+      <c r="J9" s="2">
+        <v>979.97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="2">
+        <v>64</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="2">
+        <v>5.4609999999999997E-3</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="I10" s="2">
+        <v>183.11</v>
+      </c>
+      <c r="J10" s="2">
+        <v>732.46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="3">
+        <v>5.3940000000000004E-3</v>
+      </c>
+      <c r="H11" s="3">
+        <v>46.28</v>
+      </c>
+      <c r="I11" s="3">
+        <v>185.39</v>
+      </c>
+      <c r="J11" s="3">
+        <v>741.55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="2">
         <v>8</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="6">
+      <c r="D12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="2">
         <v>0</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="6">
-        <v>3.0869999999999999E-3</v>
-      </c>
-      <c r="H7" s="6">
-        <v>323.97000000000003</v>
-      </c>
-      <c r="I7" s="6">
-        <v>1295.8800000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6">
+      <c r="F12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2.9290000000000002E-3</v>
+      </c>
+      <c r="H12" s="2">
+        <v>42.61</v>
+      </c>
+      <c r="I12" s="2">
+        <v>341.38</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1365.51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="2">
         <v>16</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="6">
+      <c r="D13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="2">
         <v>0</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="6">
-        <v>3.3930000000000002E-3</v>
-      </c>
-      <c r="H8" s="6">
-        <v>294.7</v>
-      </c>
-      <c r="I8" s="6">
-        <v>1178.81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6">
+      <c r="F13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="2">
+        <v>3.0769999999999999E-3</v>
+      </c>
+      <c r="H13" s="2">
+        <v>20.36</v>
+      </c>
+      <c r="I13" s="2">
+        <v>325.02999999999997</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1300.1099999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="2">
         <v>32</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="6">
+      <c r="D14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="2">
         <v>0</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="6">
-        <v>4.0819999999999997E-3</v>
-      </c>
-      <c r="H9" s="6">
-        <v>244.99</v>
-      </c>
-      <c r="I9" s="6">
-        <v>979.97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6">
+      <c r="F14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="2">
+        <v>3.4290000000000002E-3</v>
+      </c>
+      <c r="H14" s="2">
+        <v>9.2899999999999991</v>
+      </c>
+      <c r="I14" s="2">
+        <v>291.58999999999997</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1166.3599999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="2">
         <v>64</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="6">
-        <v>5.4609999999999997E-3</v>
-      </c>
-      <c r="H10" s="6">
-        <v>183.11</v>
-      </c>
-      <c r="I10" s="6">
-        <v>732.46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5">
-        <v>2</v>
-      </c>
-      <c r="C11" s="6">
-        <v>4</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="6">
-        <v>0</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="7">
-        <v>5.3940000000000004E-3</v>
-      </c>
-      <c r="H11" s="7">
-        <v>185.39</v>
-      </c>
-      <c r="I11" s="7">
-        <v>741.55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6">
-        <v>8</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="6">
-        <v>0</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="6">
-        <v>2.9290000000000002E-3</v>
-      </c>
-      <c r="H12" s="6">
-        <v>341.38</v>
-      </c>
-      <c r="I12" s="6">
-        <v>1365.51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6">
-        <v>16</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="6">
-        <v>0</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="6">
-        <v>3.0769999999999999E-3</v>
-      </c>
-      <c r="H13" s="6">
-        <v>325.02999999999997</v>
-      </c>
-      <c r="I13" s="6">
-        <v>1300.1099999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6">
-        <v>32</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="6">
-        <v>0</v>
-      </c>
-      <c r="F14" s="6" t="s">
+      <c r="D15" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="6">
-        <v>3.4290000000000002E-3</v>
-      </c>
-      <c r="H14" s="6">
-        <v>291.58999999999997</v>
-      </c>
-      <c r="I14" s="6">
-        <v>1166.3599999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6">
-        <v>64</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
     <mergeCell ref="B11:B15"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A15"/>
-    <mergeCell ref="A3:I3"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="G4:G5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
     <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="D15:J15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated with ruby multi-pumping report and finished the window summation experiment
</commit_message>
<xml_diff>
--- a/assets/data/multipumping.xlsx
+++ b/assets/data/multipumping.xlsx
@@ -83,6 +83,41 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>10163(3.41%)</t>
+  </si>
+  <si>
+    <t>45(2.11%)</t>
+  </si>
+  <si>
+    <t>12656(4.25%)</t>
+  </si>
+  <si>
+    <t>68(3.20%)</t>
+  </si>
+  <si>
+    <t>17082(5.74%)</t>
+  </si>
+  <si>
+    <t>117(5.50%)</t>
+  </si>
+  <si>
+    <t>28260(9.50%)</t>
+  </si>
+  <si>
+    <t>205(9.63%)</t>
+  </si>
+  <si>
+    <t>FAILED TO MEET TIMING!</t>
+  </si>
+  <si>
+    <t>Freq per elem
+(MHz)</t>
+  </si>
+  <si>
+    <t>Freq per tick
+(MHz)</t>
   </si>
   <si>
     <r>
@@ -124,49 +159,17 @@
         <rFont val="Consolas"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> value</t>
+      <t xml:space="preserve"> value (Stream Frequency=100MHz)</t>
     </r>
-  </si>
-  <si>
-    <t>10163(3.41%)</t>
-  </si>
-  <si>
-    <t>45(2.11%)</t>
-  </si>
-  <si>
-    <t>12656(4.25%)</t>
-  </si>
-  <si>
-    <t>68(3.20%)</t>
-  </si>
-  <si>
-    <t>17082(5.74%)</t>
-  </si>
-  <si>
-    <t>117(5.50%)</t>
-  </si>
-  <si>
-    <t>28260(9.50%)</t>
-  </si>
-  <si>
-    <t>205(9.63%)</t>
-  </si>
-  <si>
-    <t>FAILED TO MEET TIMING!</t>
-  </si>
-  <si>
-    <t>Freq per elem
-(MHz)</t>
-  </si>
-  <si>
-    <t>Freq per tick
-(MHz)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -236,28 +239,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,7 +547,7 @@
   <dimension ref="A3:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -554,7 +560,7 @@
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -567,37 +573,37 @@
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="7" t="s">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="7" t="s">
+      <c r="H4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="I4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
@@ -607,17 +613,17 @@
       <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <f>8192*8192</f>
         <v>67108864</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>1</v>
       </c>
       <c r="C6" s="2">
@@ -632,22 +638,22 @@
       <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="2">
-        <v>2.9940000000000001E-3</v>
-      </c>
-      <c r="H6" s="2">
-        <v>83.51</v>
-      </c>
-      <c r="I6" s="2">
-        <v>333.96</v>
-      </c>
-      <c r="J6" s="2">
-        <v>1335.84</v>
+      <c r="G6" s="8">
+        <v>2.7750000000000001E-3</v>
+      </c>
+      <c r="H6" s="10">
+        <v>90.1</v>
+      </c>
+      <c r="I6" s="10">
+        <v>360.4</v>
+      </c>
+      <c r="J6" s="10">
+        <v>1441.61</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="2">
         <v>8</v>
       </c>
@@ -660,22 +666,22 @@
       <c r="F7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="2">
-        <v>3.0869999999999999E-3</v>
-      </c>
-      <c r="H7" s="2">
-        <v>40.369999999999997</v>
-      </c>
-      <c r="I7" s="2">
-        <v>323.97000000000003</v>
-      </c>
-      <c r="J7" s="2">
-        <v>1295.8800000000001</v>
+      <c r="G7" s="8">
+        <v>2.7130000000000001E-3</v>
+      </c>
+      <c r="H7" s="10">
+        <v>46.08</v>
+      </c>
+      <c r="I7" s="10">
+        <v>368.65</v>
+      </c>
+      <c r="J7" s="10">
+        <v>1474.61</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
       <c r="C8" s="2">
         <v>16</v>
       </c>
@@ -688,22 +694,22 @@
       <c r="F8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="2">
-        <v>3.3930000000000002E-3</v>
-      </c>
-      <c r="H8" s="2">
-        <v>18.45</v>
-      </c>
-      <c r="I8" s="2">
-        <v>294.7</v>
-      </c>
-      <c r="J8" s="2">
-        <v>1178.81</v>
+      <c r="G8" s="8">
+        <v>2.686E-3</v>
+      </c>
+      <c r="H8" s="10">
+        <v>23.27</v>
+      </c>
+      <c r="I8" s="10">
+        <v>372.29</v>
+      </c>
+      <c r="J8" s="10">
+        <v>1489.15</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
       <c r="C9" s="2">
         <v>32</v>
       </c>
@@ -716,22 +722,22 @@
       <c r="F9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="2">
-        <v>4.0819999999999997E-3</v>
-      </c>
-      <c r="H9" s="2">
-        <v>7.67</v>
-      </c>
-      <c r="I9" s="2">
-        <v>244.99</v>
-      </c>
-      <c r="J9" s="2">
-        <v>979.97</v>
+      <c r="G9" s="8">
+        <v>2.66E-3</v>
+      </c>
+      <c r="H9" s="10">
+        <v>11.75</v>
+      </c>
+      <c r="I9" s="10">
+        <v>375.93</v>
+      </c>
+      <c r="J9" s="10">
+        <v>1503.72</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="2">
         <v>64</v>
       </c>
@@ -744,151 +750,156 @@
       <c r="F10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="2">
-        <v>5.4609999999999997E-3</v>
-      </c>
-      <c r="H10" s="2">
+      <c r="G10" s="8">
+        <v>2.6589999999999999E-3</v>
+      </c>
+      <c r="H10" s="10">
         <v>2.9</v>
       </c>
-      <c r="I10" s="2">
-        <v>183.11</v>
-      </c>
-      <c r="J10" s="2">
-        <v>732.46</v>
+      <c r="I10" s="10">
+        <v>376.12</v>
+      </c>
+      <c r="J10" s="10">
+        <v>1504.5</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3">
         <v>2</v>
       </c>
       <c r="C11" s="2">
         <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="2">
         <v>0</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="3">
-        <v>5.3940000000000004E-3</v>
-      </c>
-      <c r="H11" s="3">
-        <v>46.28</v>
-      </c>
-      <c r="I11" s="3">
-        <v>185.39</v>
-      </c>
-      <c r="J11" s="3">
-        <v>741.55</v>
+        <v>20</v>
+      </c>
+      <c r="G11" s="9">
+        <v>5.2750000000000002E-3</v>
+      </c>
+      <c r="H11" s="11">
+        <v>47.39</v>
+      </c>
+      <c r="I11" s="11">
+        <v>189.58</v>
+      </c>
+      <c r="J11" s="11">
+        <v>758.32</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
       <c r="C12" s="2">
         <v>8</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" s="2">
         <v>0</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="2">
-        <v>2.9290000000000002E-3</v>
-      </c>
-      <c r="H12" s="2">
-        <v>42.61</v>
-      </c>
-      <c r="I12" s="2">
-        <v>341.38</v>
-      </c>
-      <c r="J12" s="2">
-        <v>1365.51</v>
+        <v>22</v>
+      </c>
+      <c r="G12" s="8">
+        <v>2.7160000000000001E-3</v>
+      </c>
+      <c r="H12" s="10">
+        <v>46.03</v>
+      </c>
+      <c r="I12" s="10">
+        <v>368.23</v>
+      </c>
+      <c r="J12" s="10">
+        <v>1472.9</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
       <c r="C13" s="2">
         <v>16</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" s="2">
         <v>0</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="2">
-        <v>3.0769999999999999E-3</v>
-      </c>
-      <c r="H13" s="2">
-        <v>20.36</v>
-      </c>
-      <c r="I13" s="2">
-        <v>325.02999999999997</v>
-      </c>
-      <c r="J13" s="2">
-        <v>1300.1099999999999</v>
+        <v>24</v>
+      </c>
+      <c r="G13" s="8">
+        <v>2.6770000000000001E-3</v>
+      </c>
+      <c r="H13" s="10">
+        <v>23.35</v>
+      </c>
+      <c r="I13" s="10">
+        <v>373.55</v>
+      </c>
+      <c r="J13" s="10">
+        <v>1494.22</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
       <c r="C14" s="2">
         <v>32</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" s="2">
         <v>0</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="2">
-        <v>3.4290000000000002E-3</v>
-      </c>
-      <c r="H14" s="2">
-        <v>9.2899999999999991</v>
-      </c>
-      <c r="I14" s="2">
-        <v>291.58999999999997</v>
-      </c>
-      <c r="J14" s="2">
-        <v>1166.3599999999999</v>
+        <v>26</v>
+      </c>
+      <c r="G14" s="8">
+        <v>2.6679999999999998E-3</v>
+      </c>
+      <c r="H14" s="10">
+        <v>11.71</v>
+      </c>
+      <c r="I14" s="10">
+        <v>374.87</v>
+      </c>
+      <c r="J14" s="10">
+        <v>1499.47</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
       <c r="C15" s="2">
         <v>64</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
+      <c r="D15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="A3:J3"/>
     <mergeCell ref="B11:B15"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="A4:A5"/>
@@ -896,11 +907,6 @@
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="A3:J3"/>
     <mergeCell ref="D15:J15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>